<commit_message>
Update bug report and add testing file
Update the bug report.xlsx
Add testing for load and save button
</commit_message>
<xml_diff>
--- a/Documentation/Bug report.xlsx
+++ b/Documentation/Bug report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsn19012\Downloads\Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsn19012\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6700BC0C-0D9C-4BE9-B1BA-0F24657A2685}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4C6C0E-C646-4944-B974-CB89B598B168}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" xr2:uid="{1D6639C1-7F7F-4588-BDE1-D20B3C8430F2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">Expected result: </t>
   </si>
@@ -60,9 +60,6 @@
     <t>[Enter the actual result.]</t>
   </si>
   <si>
-    <t>[Enter the actual result. ]</t>
-  </si>
-  <si>
     <t>Fixed</t>
   </si>
   <si>
@@ -76,6 +73,23 @@
   </si>
   <si>
     <t>Date for last update:</t>
+  </si>
+  <si>
+    <t>InitialPos in Robot_YUMI.py</t>
+  </si>
+  <si>
+    <t>50024: Corner path failure
+Description
+Task: T_ROB1.Corner path executed as stop point due to some of the following reasons:          • Time delay. • Closely programmed points. • System requires high CPU load.Program ref. /SERVER/main/MoveAbsJ/377.</t>
+  </si>
+  <si>
+    <t>Jiantao Shen</t>
+  </si>
+  <si>
+    <t>Disconnect the robotic arm Yumi.</t>
+  </si>
+  <si>
+    <t>The robot arm should set all joints to specific angles.</t>
   </si>
 </sst>
 </file>
@@ -187,7 +201,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -206,6 +220,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -528,7 +545,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,7 +568,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>8</v>
@@ -563,10 +580,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>2</v>
@@ -596,31 +613,31 @@
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="223.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>5</v>
+        <v>18</v>
+      </c>
+      <c r="F3" s="7">
+        <v>45198</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update with newest Yumi Code
This code is for try if the GUI is possible to run in the simulation
</commit_message>
<xml_diff>
--- a/Documentation/Bug report.xlsx
+++ b/Documentation/Bug report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsn19012\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsn19012\Downloads\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4C6C0E-C646-4944-B974-CB89B598B168}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6700BC0C-0D9C-4BE9-B1BA-0F24657A2685}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" xr2:uid="{1D6639C1-7F7F-4588-BDE1-D20B3C8430F2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t xml:space="preserve">Expected result: </t>
   </si>
@@ -60,6 +60,9 @@
     <t>[Enter the actual result.]</t>
   </si>
   <si>
+    <t>[Enter the actual result. ]</t>
+  </si>
+  <si>
     <t>Fixed</t>
   </si>
   <si>
@@ -73,23 +76,6 @@
   </si>
   <si>
     <t>Date for last update:</t>
-  </si>
-  <si>
-    <t>InitialPos in Robot_YUMI.py</t>
-  </si>
-  <si>
-    <t>50024: Corner path failure
-Description
-Task: T_ROB1.Corner path executed as stop point due to some of the following reasons:          • Time delay. • Closely programmed points. • System requires high CPU load.Program ref. /SERVER/main/MoveAbsJ/377.</t>
-  </si>
-  <si>
-    <t>Jiantao Shen</t>
-  </si>
-  <si>
-    <t>Disconnect the robotic arm Yumi.</t>
-  </si>
-  <si>
-    <t>The robot arm should set all joints to specific angles.</t>
   </si>
 </sst>
 </file>
@@ -201,7 +187,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -220,9 +206,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -545,7 +528,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection sqref="A1:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,7 +551,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>8</v>
@@ -580,10 +563,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>2</v>
@@ -613,31 +596,31 @@
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="223.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="7">
-        <v>45198</v>
+        <v>4</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>